<commit_message>
Steel_Dwass_1 and loginom_feature_importance working
</commit_message>
<xml_diff>
--- a/column_analysis_results.xlsx
+++ b/column_analysis_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,17 +481,23 @@
       <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1.469072164948454</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.5003337383062596</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +505,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.62303664921466</v>
+        <v>1.469072164948454</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7285842029271764</v>
+        <v>0.5003337383062596</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -516,33 +522,39 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.455497382198953</v>
+        <v>1.62303664921466</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4993244264882782</v>
+        <v>0.7285842029271764</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
-        <v>1.172774869109948</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.3790460971783868</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -550,16 +562,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.830687830687831</v>
+        <v>1.455497382198953</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9636533172576941</v>
+        <v>0.4993244264882782</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -567,16 +579,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1.44559585492228</v>
+        <v>1.172774869109948</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6110047926566498</v>
+        <v>0.3790460971783868</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -584,67 +596,85 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.036649214659686</v>
+        <v>1.830687830687831</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1883928635560638</v>
+        <v>0.9636533172576941</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -652,16 +682,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>1.44559585492228</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.6110047926566498</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -669,10 +699,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.026178010471204</v>
+        <v>1.036649214659686</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1600840231293682</v>
+        <v>0.1883928635560638</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
@@ -686,16 +716,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1.020942408376963</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1435678890665016</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -703,16 +733,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>13.4869109947644</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>1.3450049451815</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -720,16 +750,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1.93717277486911</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2432896616492725</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -737,16 +767,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1.895287958115183</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3069867060579905</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -754,10 +784,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1.931937172774869</v>
+        <v>1.026178010471204</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2525155883262541</v>
+        <v>0.1600840231293682</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
@@ -771,10 +801,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1.015706806282723</v>
+        <v>1.020942408376963</v>
       </c>
       <c r="C20" t="n">
-        <v>0.124665438192574</v>
+        <v>0.1435678890665016</v>
       </c>
       <c r="D20" t="n">
         <v>1</v>
@@ -788,16 +818,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1.43979057591623</v>
+        <v>13.4869109947644</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4976660877115174</v>
+        <v>1.3450049451815</v>
       </c>
       <c r="D21" t="n">
         <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
@@ -805,16 +835,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>18.00529100529101</v>
+        <v>1.93717277486911</v>
       </c>
       <c r="C22" t="n">
-        <v>1.961049855869529</v>
+        <v>0.2432896616492725</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -822,16 +852,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>2.387434554973822</v>
+        <v>1.895287958115183</v>
       </c>
       <c r="C23" t="n">
-        <v>1.527519218471463</v>
+        <v>0.3069867060579905</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -839,10 +869,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1.141361256544503</v>
+        <v>1.931937172774869</v>
       </c>
       <c r="C24" t="n">
-        <v>0.349309439603781</v>
+        <v>0.2525155883262541</v>
       </c>
       <c r="D24" t="n">
         <v>1</v>
@@ -855,34 +885,46 @@
       <c r="A25" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="n">
-        <v>1.115183246073298</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.3200819680084218</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="n">
-        <v>1.083769633507853</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.2777701232832868</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E26" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27">
@@ -890,10 +932,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1.528795811518325</v>
+        <v>1.015706806282723</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5004819941902806</v>
+        <v>0.124665438192574</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
@@ -907,10 +949,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.052356020942408</v>
+        <v>1.43979057591623</v>
       </c>
       <c r="C28" t="n">
-        <v>0.2233293507306372</v>
+        <v>0.4976660877115174</v>
       </c>
       <c r="D28" t="n">
         <v>1</v>
@@ -924,16 +966,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3333333333333333</v>
+        <v>18.00529100529101</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8164965809277259</v>
+        <v>1.961049855869529</v>
       </c>
       <c r="D29" t="n">
         <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
@@ -941,16 +983,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.151832460732984</v>
+        <v>2.387434554973822</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3598015435350837</v>
+        <v>1.527519218471463</v>
       </c>
       <c r="D30" t="n">
         <v>1</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
@@ -958,16 +1000,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.743455497382199</v>
+        <v>1.141361256544503</v>
       </c>
       <c r="C31" t="n">
-        <v>0.8778841770257917</v>
+        <v>0.349309439603781</v>
       </c>
       <c r="D31" t="n">
         <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -975,10 +1017,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.005235602094241</v>
+        <v>1.115183246073298</v>
       </c>
       <c r="C32" t="n">
-        <v>0.07235746052924216</v>
+        <v>0.3200819680084218</v>
       </c>
       <c r="D32" t="n">
         <v>1</v>
@@ -992,10 +1034,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1.026178010471204</v>
+        <v>1.083769633507853</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1600840231293682</v>
+        <v>0.2777701232832868</v>
       </c>
       <c r="D33" t="n">
         <v>1</v>
@@ -1009,16 +1051,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>10.40732984293194</v>
+        <v>1.528795811518325</v>
       </c>
       <c r="C34" t="n">
-        <v>4.721523916691959</v>
+        <v>0.5004819941902806</v>
       </c>
       <c r="D34" t="n">
         <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>87</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -1026,10 +1068,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1.612565445026178</v>
+        <v>1.052356020942408</v>
       </c>
       <c r="C35" t="n">
-        <v>0.4884445932697035</v>
+        <v>0.2233293507306372</v>
       </c>
       <c r="D35" t="n">
         <v>1</v>
@@ -1043,16 +1085,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.952879581151832</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C36" t="n">
-        <v>1.319042547955796</v>
+        <v>0.8164965809277259</v>
       </c>
       <c r="D36" t="n">
         <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -1060,10 +1102,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1.471204188481675</v>
+        <v>1.151832460732984</v>
       </c>
       <c r="C37" t="n">
-        <v>0.5004819941902806</v>
+        <v>0.3598015435350837</v>
       </c>
       <c r="D37" t="n">
         <v>1</v>
@@ -1077,16 +1119,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>2.418848167539267</v>
+        <v>0.743455497382199</v>
       </c>
       <c r="C38" t="n">
-        <v>1.539808851084511</v>
+        <v>0.8778841770257917</v>
       </c>
       <c r="D38" t="n">
         <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -1094,10 +1136,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1.258241758241758</v>
+        <v>1.005235602094241</v>
       </c>
       <c r="C39" t="n">
-        <v>0.4388749892021278</v>
+        <v>0.07235746052924216</v>
       </c>
       <c r="D39" t="n">
         <v>1</v>
@@ -1111,16 +1153,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>3.445054945054945</v>
+        <v>1.026178010471204</v>
       </c>
       <c r="C40" t="n">
-        <v>1.747848795327846</v>
+        <v>0.1600840231293682</v>
       </c>
       <c r="D40" t="n">
         <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1128,16 +1170,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>2.174603174603174</v>
+        <v>10.40732984293194</v>
       </c>
       <c r="C41" t="n">
-        <v>0.9028268113356316</v>
+        <v>4.721523916691959</v>
       </c>
       <c r="D41" t="n">
         <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42">
@@ -1145,10 +1187,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>14.93157894736842</v>
+        <v>1.612565445026178</v>
       </c>
       <c r="C42" t="n">
-        <v>0.9431191251430153</v>
+        <v>0.4884445932697035</v>
       </c>
       <c r="D42" t="n">
         <v>1</v>
@@ -1162,16 +1204,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>36.41780104712043</v>
+        <v>1.952879581151832</v>
       </c>
       <c r="C43" t="n">
-        <v>0.2515162068628724</v>
+        <v>1.319042547955796</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -1179,16 +1221,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1.41578947368421</v>
+        <v>1.471204188481675</v>
       </c>
       <c r="C44" t="n">
-        <v>0.7703247153534526</v>
+        <v>0.5004819941902806</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
@@ -1196,16 +1238,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>2.418848167539267</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>1.539808851084511</v>
       </c>
       <c r="D45" t="n">
         <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46">
@@ -1213,16 +1255,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>1.258241758241758</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>0.4388749892021278</v>
       </c>
       <c r="D46" t="n">
         <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -1230,16 +1272,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1.235602094240838</v>
+        <v>3.445054945054945</v>
       </c>
       <c r="C47" t="n">
-        <v>0.4254898462463575</v>
+        <v>1.747848795327846</v>
       </c>
       <c r="D47" t="n">
         <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48">
@@ -1247,16 +1289,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>122.2146596858639</v>
+        <v>2.174603174603174</v>
       </c>
       <c r="C48" t="n">
-        <v>15.01406339909346</v>
+        <v>0.9028268113356316</v>
       </c>
       <c r="D48" t="n">
         <v>1</v>
       </c>
       <c r="E48" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49">
@@ -1264,16 +1306,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>79.282722513089</v>
+        <v>14.93157894736842</v>
       </c>
       <c r="C49" t="n">
-        <v>11.19415566132454</v>
+        <v>0.9431191251430153</v>
       </c>
       <c r="D49" t="n">
         <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -1281,33 +1323,39 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1.31413612565445</v>
+        <v>36.41780104712043</v>
       </c>
       <c r="C50" t="n">
-        <v>0.4653907948150615</v>
+        <v>0.2515162068628724</v>
       </c>
       <c r="D50" t="n">
         <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="n">
-        <v>1.026315789473684</v>
-      </c>
-      <c r="C51" t="n">
-        <v>0.160495612240071</v>
-      </c>
-      <c r="D51" t="n">
-        <v>1</v>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52">
@@ -1315,16 +1363,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>1.036842105263158</v>
+        <v>1.41578947368421</v>
       </c>
       <c r="C52" t="n">
-        <v>0.1888716882433231</v>
+        <v>0.7703247153534526</v>
       </c>
       <c r="D52" t="n">
         <v>1</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
@@ -1332,16 +1380,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>106.4607329842932</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
-        <v>10.24578359937245</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
         <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -1349,16 +1397,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>34.58115183246073</v>
+        <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>4.624017475493327</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
         <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -1366,33 +1414,39 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>1.235602094240838</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>0.4254898462463575</v>
       </c>
       <c r="D55" t="n">
         <v>1</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="n">
-        <v>1.042553191489362</v>
-      </c>
-      <c r="C56" t="n">
-        <v>0.2023864898484639</v>
-      </c>
-      <c r="D56" t="n">
-        <v>1</v>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E56" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57">
@@ -1400,16 +1454,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>122.2146596858639</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>15.01406339909346</v>
       </c>
       <c r="D57" t="n">
         <v>1</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58">
@@ -1417,16 +1471,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>141.9162303664922</v>
+        <v>79.282722513089</v>
       </c>
       <c r="C58" t="n">
-        <v>4.838801333662292</v>
+        <v>11.19415566132454</v>
       </c>
       <c r="D58" t="n">
         <v>1</v>
       </c>
       <c r="E58" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59">
@@ -1434,10 +1488,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>1.010471204188482</v>
+        <v>1.31413612565445</v>
       </c>
       <c r="C59" t="n">
-        <v>0.1020592601751045</v>
+        <v>0.4653907948150615</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
@@ -1451,10 +1505,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>1.041884816753927</v>
+        <v>1.026315789473684</v>
       </c>
       <c r="C60" t="n">
-        <v>0.2008524132943153</v>
+        <v>0.160495612240071</v>
       </c>
       <c r="D60" t="n">
         <v>1</v>
@@ -1468,16 +1522,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>1.06282722513089</v>
+        <v>1.036842105263158</v>
       </c>
       <c r="C61" t="n">
-        <v>0.301278619941473</v>
+        <v>0.1888716882433231</v>
       </c>
       <c r="D61" t="n">
         <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
@@ -1485,16 +1539,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>1.612565445026178</v>
+        <v>106.4607329842932</v>
       </c>
       <c r="C62" t="n">
-        <v>0.4884445932697035</v>
+        <v>10.24578359937245</v>
       </c>
       <c r="D62" t="n">
         <v>1</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63">
@@ -1502,16 +1556,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>2.142076502732241</v>
+        <v>34.58115183246073</v>
       </c>
       <c r="C63" t="n">
-        <v>0.7785094624512687</v>
+        <v>4.624017475493327</v>
       </c>
       <c r="D63" t="n">
         <v>1</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64">
@@ -1519,16 +1573,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>1</v>
+        <v>37.85185185185185</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>8.547170938628234</v>
       </c>
       <c r="D64" t="n">
         <v>1</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65">
@@ -1536,16 +1590,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>1.403141361256544</v>
+        <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>1.525154203046275</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
         <v>1</v>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -1553,16 +1607,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>1.62303664921466</v>
+        <v>1.042553191489362</v>
       </c>
       <c r="C66" t="n">
-        <v>0.8235310326925517</v>
+        <v>0.2023864898484639</v>
       </c>
       <c r="D66" t="n">
         <v>1</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -1570,16 +1624,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>4.373387096774193</v>
+        <v>1</v>
       </c>
       <c r="C67" t="n">
-        <v>0.8525407690308036</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E67" t="n">
-        <v>120</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1587,16 +1641,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>64.13617021276595</v>
+        <v>141.9162303664922</v>
       </c>
       <c r="C68" t="n">
-        <v>7.081403695767067</v>
+        <v>4.838801333662292</v>
       </c>
       <c r="D68" t="n">
         <v>1</v>
       </c>
       <c r="E68" t="n">
-        <v>94</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69">
@@ -1604,16 +1658,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>8.579787234042554</v>
+        <v>1.010471204188482</v>
       </c>
       <c r="C69" t="n">
-        <v>5.118198207930701</v>
+        <v>0.1020592601751045</v>
       </c>
       <c r="D69" t="n">
         <v>1</v>
       </c>
       <c r="E69" t="n">
-        <v>91</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -1621,16 +1675,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>3.802127659574468</v>
+        <v>1.041884816753927</v>
       </c>
       <c r="C70" t="n">
-        <v>4.438780935968752</v>
+        <v>0.2008524132943153</v>
       </c>
       <c r="D70" t="n">
         <v>1</v>
       </c>
       <c r="E70" t="n">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -1638,16 +1692,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>63.11387765957446</v>
+        <v>1.06282722513089</v>
       </c>
       <c r="C71" t="n">
-        <v>12.09667438149447</v>
+        <v>0.301278619941473</v>
       </c>
       <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" t="n">
         <v>3</v>
-      </c>
-      <c r="E71" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="72">
@@ -1655,16 +1709,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>22.06595744680851</v>
+        <v>1.612565445026178</v>
       </c>
       <c r="C72" t="n">
-        <v>9.276576830276301</v>
+        <v>0.4884445932697035</v>
       </c>
       <c r="D72" t="n">
         <v>1</v>
       </c>
       <c r="E72" t="n">
-        <v>125</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -1672,16 +1726,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>17.88404255319149</v>
+        <v>2.142076502732241</v>
       </c>
       <c r="C73" t="n">
-        <v>12.74414453519766</v>
+        <v>0.7785094624512687</v>
       </c>
       <c r="D73" t="n">
         <v>1</v>
       </c>
       <c r="E73" t="n">
-        <v>135</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74">
@@ -1689,16 +1743,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>6.275132275132275</v>
+        <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>11.63260575300094</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
         <v>1</v>
       </c>
       <c r="E74" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -1706,16 +1760,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>7.158730158730159</v>
+        <v>1.403141361256544</v>
       </c>
       <c r="C75" t="n">
-        <v>13.92595122524355</v>
+        <v>1.525154203046275</v>
       </c>
       <c r="D75" t="n">
         <v>1</v>
       </c>
       <c r="E75" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76">
@@ -1723,16 +1777,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.968421052631579</v>
+        <v>1.62303664921466</v>
       </c>
       <c r="C76" t="n">
-        <v>2.005034043326535</v>
+        <v>0.8235310326925517</v>
       </c>
       <c r="D76" t="n">
         <v>1</v>
       </c>
       <c r="E76" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77">
@@ -1740,16 +1794,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>112.5294117647059</v>
+        <v>4.373387096774193</v>
       </c>
       <c r="C77" t="n">
-        <v>11.70759064386763</v>
+        <v>0.8525407690308036</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E77" t="n">
-        <v>52</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78">
@@ -1757,16 +1811,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>9.636612903225807</v>
+        <v>64.13617021276595</v>
       </c>
       <c r="C78" t="n">
-        <v>6.965578987257591</v>
+        <v>7.081403695767067</v>
       </c>
       <c r="D78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E78" t="n">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79">
@@ -1774,16 +1828,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>40.77877094972067</v>
+        <v>8.579787234042554</v>
       </c>
       <c r="C79" t="n">
-        <v>10.05719579430539</v>
+        <v>5.118198207930701</v>
       </c>
       <c r="D79" t="n">
         <v>1</v>
       </c>
       <c r="E79" t="n">
-        <v>43</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80">
@@ -1791,16 +1845,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>3.992673796791444</v>
+        <v>1.752027027027027</v>
       </c>
       <c r="C80" t="n">
-        <v>2.505288881998779</v>
+        <v>1.679345094030051</v>
       </c>
       <c r="D80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E80" t="n">
-        <v>99</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81">
@@ -1808,16 +1862,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>35.48064516129032</v>
+        <v>3.802127659574468</v>
       </c>
       <c r="C81" t="n">
-        <v>22.14469252776123</v>
+        <v>4.438780935968752</v>
       </c>
       <c r="D81" t="n">
         <v>1</v>
       </c>
       <c r="E81" t="n">
-        <v>100</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82">
@@ -1825,16 +1879,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>231.096256684492</v>
+        <v>63.11387765957446</v>
       </c>
       <c r="C82" t="n">
-        <v>64.48606865384478</v>
+        <v>12.09667438149447</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E82" t="n">
-        <v>118</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83">
@@ -1842,16 +1896,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>92.53589189189189</v>
+        <v>22.06595744680851</v>
       </c>
       <c r="C83" t="n">
-        <v>54.65198703962697</v>
+        <v>9.276576830276301</v>
       </c>
       <c r="D83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E83" t="n">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="84">
@@ -1859,16 +1913,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>29.89702702702703</v>
+        <v>17.88404255319149</v>
       </c>
       <c r="C84" t="n">
-        <v>5.206027477036294</v>
+        <v>12.74414453519766</v>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E84" t="n">
-        <v>83</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85">
@@ -1876,16 +1930,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>328.7967567567568</v>
+        <v>137.1181818181818</v>
       </c>
       <c r="C85" t="n">
-        <v>33.25952936786738</v>
+        <v>68.48572652396997</v>
       </c>
       <c r="D85" t="n">
         <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>50</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86">
@@ -1893,33 +1947,39 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>5.825268817204301</v>
+        <v>7.362585034013606</v>
       </c>
       <c r="C86" t="n">
-        <v>2.321604566928774</v>
+        <v>4.855814349607764</v>
       </c>
       <c r="D86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E86" t="n">
-        <v>148</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
         <v>85</v>
       </c>
-      <c r="B87" t="n">
-        <v>104.4724598930481</v>
-      </c>
-      <c r="C87" t="n">
-        <v>12.56554870853243</v>
-      </c>
-      <c r="D87" t="n">
-        <v>2</v>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="E87" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88">
@@ -1927,16 +1987,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>1.038882978723404</v>
+        <v>6.275132275132275</v>
       </c>
       <c r="C88" t="n">
-        <v>0.6847063675490414</v>
+        <v>11.63260575300094</v>
       </c>
       <c r="D88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E88" t="n">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89">
@@ -1944,16 +2004,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>1.194145945945946</v>
+        <v>7.158730158730159</v>
       </c>
       <c r="C89" t="n">
-        <v>1.624165453025464</v>
+        <v>13.92595122524355</v>
       </c>
       <c r="D89" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E89" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90">
@@ -1961,16 +2021,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>30.1956914893617</v>
+        <v>0.968421052631579</v>
       </c>
       <c r="C90" t="n">
-        <v>3.045668977299646</v>
+        <v>2.005034043326535</v>
       </c>
       <c r="D90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E90" t="n">
-        <v>93</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91">
@@ -1978,16 +2038,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>7.632544378698224</v>
+        <v>112.5294117647059</v>
       </c>
       <c r="C91" t="n">
-        <v>1.496446198731308</v>
+        <v>11.70759064386763</v>
       </c>
       <c r="D91" t="n">
         <v>1</v>
       </c>
       <c r="E91" t="n">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="92">
@@ -1995,16 +2055,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.7585798816568047</v>
+        <v>9.636612903225807</v>
       </c>
       <c r="C92" t="n">
-        <v>0.4151165869768628</v>
+        <v>6.965578987257591</v>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E92" t="n">
-        <v>9</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93">
@@ -2012,16 +2072,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>31.8109947643979</v>
+        <v>40.77877094972067</v>
       </c>
       <c r="C93" t="n">
-        <v>3.161234694657973</v>
+        <v>10.05719579430539</v>
       </c>
       <c r="D93" t="n">
         <v>1</v>
       </c>
       <c r="E93" t="n">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94">
@@ -2029,16 +2089,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>33.35340314136126</v>
+        <v>3.992673796791444</v>
       </c>
       <c r="C94" t="n">
-        <v>17.16883272983469</v>
+        <v>2.505288881998779</v>
       </c>
       <c r="D94" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E94" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95">
@@ -2046,16 +2106,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>6.893193717277487</v>
+        <v>35.48064516129032</v>
       </c>
       <c r="C95" t="n">
-        <v>0.8720850750159543</v>
+        <v>22.14469252776123</v>
       </c>
       <c r="D95" t="n">
         <v>1</v>
       </c>
       <c r="E95" t="n">
-        <v>34</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96">
@@ -2063,16 +2123,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>1.521052631578947</v>
+        <v>231.096256684492</v>
       </c>
       <c r="C96" t="n">
-        <v>0.5606864154538789</v>
+        <v>64.48606865384478</v>
       </c>
       <c r="D96" t="n">
         <v>1</v>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>118</v>
       </c>
     </row>
     <row r="97">
@@ -2080,16 +2140,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>2.882352941176471</v>
+        <v>92.53589189189189</v>
       </c>
       <c r="C97" t="n">
-        <v>1.476358067536468</v>
+        <v>54.65198703962697</v>
       </c>
       <c r="D97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E97" t="n">
-        <v>7</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98">
@@ -2097,16 +2157,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>1.026315789473684</v>
+        <v>29.89702702702703</v>
       </c>
       <c r="C98" t="n">
-        <v>0.1604956122400711</v>
+        <v>5.206027477036294</v>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>83</v>
       </c>
     </row>
     <row r="99">
@@ -2114,16 +2174,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>140.984126984127</v>
+        <v>328.7967567567568</v>
       </c>
       <c r="C99" t="n">
-        <v>11.33366111928392</v>
+        <v>33.25952936786738</v>
       </c>
       <c r="D99" t="n">
         <v>1</v>
       </c>
       <c r="E99" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100">
@@ -2131,16 +2191,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>8.229050279329609</v>
+        <v>22.76275862068966</v>
       </c>
       <c r="C100" t="n">
-        <v>6.038085556105598</v>
+        <v>8.102305440322272</v>
       </c>
       <c r="D100" t="n">
         <v>1</v>
       </c>
       <c r="E100" t="n">
-        <v>5</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101">
@@ -2148,16 +2208,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>8.05586592178771</v>
+        <v>6.573972602739726</v>
       </c>
       <c r="C101" t="n">
-        <v>0.7398805733501288</v>
+        <v>2.246531573245531</v>
       </c>
       <c r="D101" t="n">
         <v>1</v>
       </c>
       <c r="E101" t="n">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="102">
@@ -2165,16 +2225,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>1.017045454545455</v>
+        <v>67.75862068965517</v>
       </c>
       <c r="C102" t="n">
-        <v>0.1298100510386208</v>
+        <v>13.27038909003746</v>
       </c>
       <c r="D102" t="n">
         <v>1</v>
       </c>
       <c r="E102" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="103">
@@ -2182,16 +2242,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>50.49720670391061</v>
+        <v>234.144578313253</v>
       </c>
       <c r="C103" t="n">
-        <v>2.892015940240733</v>
+        <v>68.02781578330178</v>
       </c>
       <c r="D103" t="n">
         <v>1</v>
       </c>
       <c r="E103" t="n">
-        <v>17</v>
+        <v>68</v>
       </c>
     </row>
     <row r="104">
@@ -2199,16 +2259,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>1.089005235602094</v>
+        <v>0.1850617283950617</v>
       </c>
       <c r="C104" t="n">
-        <v>0.2854996635150049</v>
+        <v>0.1208213914916366</v>
       </c>
       <c r="D104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E104" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105">
@@ -2216,16 +2276,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>59.74853801169591</v>
+        <v>10.05</v>
       </c>
       <c r="C105" t="n">
-        <v>8.362446565204442</v>
+        <v>2.553876259848406</v>
       </c>
       <c r="D105" t="n">
         <v>1</v>
       </c>
       <c r="E105" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="106">
@@ -2233,16 +2293,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>19.56140350877193</v>
+        <v>11.49876543209877</v>
       </c>
       <c r="C106" t="n">
-        <v>4.803249673954141</v>
+        <v>7.204989483461452</v>
       </c>
       <c r="D106" t="n">
         <v>1</v>
       </c>
       <c r="E106" t="n">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="107">
@@ -2250,16 +2310,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>2.088538011695906</v>
+        <v>5.825268817204301</v>
       </c>
       <c r="C107" t="n">
-        <v>4.924395534421353</v>
+        <v>2.321604566928774</v>
       </c>
       <c r="D107" t="n">
         <v>2</v>
       </c>
       <c r="E107" t="n">
-        <v>84</v>
+        <v>148</v>
       </c>
     </row>
     <row r="108">
@@ -2267,16 +2327,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>1</v>
+        <v>14.83846153846154</v>
       </c>
       <c r="C108" t="n">
-        <v>0</v>
+        <v>12.23355226665616</v>
       </c>
       <c r="D108" t="n">
         <v>1</v>
       </c>
       <c r="E108" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="109">
@@ -2284,16 +2344,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>1.014117647058824</v>
+        <v>104.4724598930481</v>
       </c>
       <c r="C109" t="n">
-        <v>0.1709478907256341</v>
+        <v>12.56554870853243</v>
       </c>
       <c r="D109" t="n">
         <v>2</v>
       </c>
       <c r="E109" t="n">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="110">
@@ -2301,16 +2361,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>1.671823529411764</v>
+        <v>1.038882978723404</v>
       </c>
       <c r="C110" t="n">
-        <v>0.5666800162906834</v>
+        <v>0.6847063675490414</v>
       </c>
       <c r="D110" t="n">
         <v>2</v>
       </c>
       <c r="E110" t="n">
-        <v>115</v>
+        <v>41</v>
       </c>
     </row>
     <row r="111">
@@ -2318,16 +2378,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>1.769641176470588</v>
+        <v>1.194145945945946</v>
       </c>
       <c r="C111" t="n">
-        <v>0.6173065138343159</v>
+        <v>1.624165453025464</v>
       </c>
       <c r="D111" t="n">
         <v>3</v>
       </c>
       <c r="E111" t="n">
-        <v>116</v>
+        <v>43</v>
       </c>
     </row>
     <row r="112">
@@ -2335,16 +2395,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>1.07909604519774</v>
+        <v>30.1956914893617</v>
       </c>
       <c r="C112" t="n">
-        <v>0.2706542511719564</v>
+        <v>3.045668977299646</v>
       </c>
       <c r="D112" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E112" t="n">
-        <v>2</v>
+        <v>93</v>
       </c>
     </row>
     <row r="113">
@@ -2352,16 +2412,1868 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
+        <v>7.632544378698224</v>
+      </c>
+      <c r="C113" t="n">
+        <v>1.496446198731308</v>
+      </c>
+      <c r="D113" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0.7585798816568047</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0.4151165869768628</v>
+      </c>
+      <c r="D114" t="n">
+        <v>1</v>
+      </c>
+      <c r="E114" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="n">
+        <v>31.8109947643979</v>
+      </c>
+      <c r="C118" t="n">
+        <v>3.161234694657973</v>
+      </c>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="n">
+        <v>33.35340314136126</v>
+      </c>
+      <c r="C119" t="n">
+        <v>17.16883272983469</v>
+      </c>
+      <c r="D119" t="n">
+        <v>1</v>
+      </c>
+      <c r="E119" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="n">
+        <v>6.893193717277487</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0.8720850750159543</v>
+      </c>
+      <c r="D120" t="n">
+        <v>1</v>
+      </c>
+      <c r="E120" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="n">
+        <v>1.521052631578947</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0.5606864154538789</v>
+      </c>
+      <c r="D122" t="n">
+        <v>1</v>
+      </c>
+      <c r="E122" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="n">
+        <v>2.882352941176471</v>
+      </c>
+      <c r="C124" t="n">
+        <v>1.476358067536468</v>
+      </c>
+      <c r="D124" t="n">
+        <v>1</v>
+      </c>
+      <c r="E124" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="n">
+        <v>1.026315789473684</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0.1604956122400711</v>
+      </c>
+      <c r="D125" t="n">
+        <v>1</v>
+      </c>
+      <c r="E125" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="n">
+        <v>140.984126984127</v>
+      </c>
+      <c r="C128" t="n">
+        <v>11.33366111928392</v>
+      </c>
+      <c r="D128" t="n">
+        <v>1</v>
+      </c>
+      <c r="E128" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="n">
+        <v>41.18150943396226</v>
+      </c>
+      <c r="C129" t="n">
+        <v>23.83766253998285</v>
+      </c>
+      <c r="D129" t="n">
+        <v>2</v>
+      </c>
+      <c r="E129" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="n">
+        <v>8.229050279329609</v>
+      </c>
+      <c r="C130" t="n">
+        <v>6.038085556105598</v>
+      </c>
+      <c r="D130" t="n">
+        <v>1</v>
+      </c>
+      <c r="E130" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="n">
+        <v>8.05586592178771</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0.7398805733501288</v>
+      </c>
+      <c r="D131" t="n">
+        <v>1</v>
+      </c>
+      <c r="E131" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="n">
+        <v>1.017045454545455</v>
+      </c>
+      <c r="C132" t="n">
+        <v>0.1298100510386208</v>
+      </c>
+      <c r="D132" t="n">
+        <v>1</v>
+      </c>
+      <c r="E132" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="n">
+        <v>50.49720670391061</v>
+      </c>
+      <c r="C134" t="n">
+        <v>2.892015940240733</v>
+      </c>
+      <c r="D134" t="n">
+        <v>1</v>
+      </c>
+      <c r="E134" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="n">
+        <v>1.089005235602094</v>
+      </c>
+      <c r="C135" t="n">
+        <v>0.2854996635150049</v>
+      </c>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
+      <c r="E135" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="n">
+        <v>59.74853801169591</v>
+      </c>
+      <c r="C136" t="n">
+        <v>8.362446565204442</v>
+      </c>
+      <c r="D136" t="n">
+        <v>1</v>
+      </c>
+      <c r="E136" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="n">
+        <v>19.56140350877193</v>
+      </c>
+      <c r="C137" t="n">
+        <v>4.803249673954141</v>
+      </c>
+      <c r="D137" t="n">
+        <v>1</v>
+      </c>
+      <c r="E137" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="n">
+        <v>2.088538011695906</v>
+      </c>
+      <c r="C138" t="n">
+        <v>4.924395534421353</v>
+      </c>
+      <c r="D138" t="n">
+        <v>2</v>
+      </c>
+      <c r="E138" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="n">
+        <v>1</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>1</v>
+      </c>
+      <c r="E139" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="n">
+        <v>1.014117647058824</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.1709478907256341</v>
+      </c>
+      <c r="D140" t="n">
+        <v>2</v>
+      </c>
+      <c r="E140" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="n">
+        <v>1.671823529411764</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0.5666800162906834</v>
+      </c>
+      <c r="D141" t="n">
+        <v>2</v>
+      </c>
+      <c r="E141" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="n">
+        <v>1.769641176470588</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0.6173065138343159</v>
+      </c>
+      <c r="D142" t="n">
+        <v>3</v>
+      </c>
+      <c r="E142" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="n">
+        <v>1.07909604519774</v>
+      </c>
+      <c r="C145" t="n">
+        <v>0.2706542511719564</v>
+      </c>
+      <c r="D145" t="n">
+        <v>1</v>
+      </c>
+      <c r="E145" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="n">
         <v>1.016949152542373</v>
       </c>
-      <c r="C113" t="n">
+      <c r="C146" t="n">
         <v>0.1294470877857418</v>
       </c>
-      <c r="D113" t="n">
-        <v>1</v>
-      </c>
-      <c r="E113" t="n">
-        <v>2</v>
+      <c r="D146" t="n">
+        <v>1</v>
+      </c>
+      <c r="E146" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="n">
+        <v>0.7154098360655737</v>
+      </c>
+      <c r="C147" t="n">
+        <v>0.2822916563325467</v>
+      </c>
+      <c r="D147" t="n">
+        <v>2</v>
+      </c>
+      <c r="E147" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="n">
+        <v>2.029180327868853</v>
+      </c>
+      <c r="C148" t="n">
+        <v>10.02341596713781</v>
+      </c>
+      <c r="D148" t="n">
+        <v>2</v>
+      </c>
+      <c r="E148" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="n">
+        <v>0.7286885245901641</v>
+      </c>
+      <c r="C149" t="n">
+        <v>0.2358846851736109</v>
+      </c>
+      <c r="D149" t="n">
+        <v>2</v>
+      </c>
+      <c r="E149" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="n">
+        <v>1.470588235294118</v>
+      </c>
+      <c r="C150" t="n">
+        <v>0.531699281950512</v>
+      </c>
+      <c r="D150" t="n">
+        <v>1</v>
+      </c>
+      <c r="E150" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="n">
+        <v>2.90625</v>
+      </c>
+      <c r="C151" t="n">
+        <v>1.891658800067553</v>
+      </c>
+      <c r="D151" t="n">
+        <v>1</v>
+      </c>
+      <c r="E151" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="n">
+        <v>30.3004347826087</v>
+      </c>
+      <c r="C154" t="n">
+        <v>8.481556087709084</v>
+      </c>
+      <c r="D154" t="n">
+        <v>2</v>
+      </c>
+      <c r="E154" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="n">
+        <v>13.99269565217391</v>
+      </c>
+      <c r="C155" t="n">
+        <v>62.52947182072219</v>
+      </c>
+      <c r="D155" t="n">
+        <v>2</v>
+      </c>
+      <c r="E155" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="n">
+        <v>28.22843478260869</v>
+      </c>
+      <c r="C156" t="n">
+        <v>11.04819081730677</v>
+      </c>
+      <c r="D156" t="n">
+        <v>2</v>
+      </c>
+      <c r="E156" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="n">
+        <v>30.3004347826087</v>
+      </c>
+      <c r="C157" t="n">
+        <v>8.481556087709084</v>
+      </c>
+      <c r="D157" t="n">
+        <v>2</v>
+      </c>
+      <c r="E157" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="n">
+        <v>15.00234782608696</v>
+      </c>
+      <c r="C158" t="n">
+        <v>4.21625828348353</v>
+      </c>
+      <c r="D158" t="n">
+        <v>2</v>
+      </c>
+      <c r="E158" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="n">
+        <v>0.6870434782608695</v>
+      </c>
+      <c r="C159" t="n">
+        <v>1.583446149579888</v>
+      </c>
+      <c r="D159" t="n">
+        <v>2</v>
+      </c>
+      <c r="E159" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="n">
+        <v>18.69791304347826</v>
+      </c>
+      <c r="C160" t="n">
+        <v>15.11296251425526</v>
+      </c>
+      <c r="D160" t="n">
+        <v>2</v>
+      </c>
+      <c r="E160" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="n">
+        <v>27.96260869565217</v>
+      </c>
+      <c r="C161" t="n">
+        <v>11.27337657717513</v>
+      </c>
+      <c r="D161" t="n">
+        <v>2</v>
+      </c>
+      <c r="E161" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="n">
+        <v>2.695478260869566</v>
+      </c>
+      <c r="C162" t="n">
+        <v>1.144113265370588</v>
+      </c>
+      <c r="D162" t="n">
+        <v>2</v>
+      </c>
+      <c r="E162" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="n">
+        <v>2.067217391304348</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0.6997186750804162</v>
+      </c>
+      <c r="D163" t="n">
+        <v>2</v>
+      </c>
+      <c r="E163" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="C164" t="n">
+        <v>0.4449896509736875</v>
+      </c>
+      <c r="D164" t="n">
+        <v>2</v>
+      </c>
+      <c r="E164" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="n">
+        <v>1.708782608695652</v>
+      </c>
+      <c r="C165" t="n">
+        <v>9.155864303086682</v>
+      </c>
+      <c r="D165" t="n">
+        <v>2</v>
+      </c>
+      <c r="E165" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="n">
+        <v>1.467826086956522</v>
+      </c>
+      <c r="C166" t="n">
+        <v>6.926169897076822</v>
+      </c>
+      <c r="D166" t="n">
+        <v>2</v>
+      </c>
+      <c r="E166" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="n">
+        <v>7.634834782608696</v>
+      </c>
+      <c r="C167" t="n">
+        <v>8.273837909529382</v>
+      </c>
+      <c r="D167" t="n">
+        <v>3</v>
+      </c>
+      <c r="E167" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="n">
+        <v>98.69713043478261</v>
+      </c>
+      <c r="C169" t="n">
+        <v>55.17866827789009</v>
+      </c>
+      <c r="D169" t="n">
+        <v>2</v>
+      </c>
+      <c r="E169" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="n">
+        <v>31.94173913043478</v>
+      </c>
+      <c r="C170" t="n">
+        <v>9.287569343876525</v>
+      </c>
+      <c r="D170" t="n">
+        <v>1</v>
+      </c>
+      <c r="E170" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="n">
+        <v>68.96086956521739</v>
+      </c>
+      <c r="C171" t="n">
+        <v>16.82553768934203</v>
+      </c>
+      <c r="D171" t="n">
+        <v>1</v>
+      </c>
+      <c r="E171" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="n">
+        <v>-1.210260869565217</v>
+      </c>
+      <c r="C172" t="n">
+        <v>5.331701032153097</v>
+      </c>
+      <c r="D172" t="n">
+        <v>2</v>
+      </c>
+      <c r="E172" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="n">
+        <v>31.05739130434782</v>
+      </c>
+      <c r="C173" t="n">
+        <v>9.605938047197181</v>
+      </c>
+      <c r="D173" t="n">
+        <v>1</v>
+      </c>
+      <c r="E173" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="n">
+        <v>33.4991452991453</v>
+      </c>
+      <c r="C174" t="n">
+        <v>10.62851966633508</v>
+      </c>
+      <c r="D174" t="n">
+        <v>1</v>
+      </c>
+      <c r="E174" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="n">
+        <v>1.148936170212766</v>
+      </c>
+      <c r="C175" t="n">
+        <v>0.9320086630558218</v>
+      </c>
+      <c r="D175" t="n">
+        <v>1</v>
+      </c>
+      <c r="E175" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="n">
+        <v>0.3829787234042553</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0.491368607293056</v>
+      </c>
+      <c r="D176" t="n">
+        <v>1</v>
+      </c>
+      <c r="E176" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="C177" t="n">
+        <v>0.4767312946227962</v>
+      </c>
+      <c r="D177" t="n">
+        <v>1</v>
+      </c>
+      <c r="E177" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="n">
+        <v>1.404255319148936</v>
+      </c>
+      <c r="C178" t="n">
+        <v>0.924534535486938</v>
+      </c>
+      <c r="D178" t="n">
+        <v>1</v>
+      </c>
+      <c r="E178" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="n">
+        <v>0.4042553191489361</v>
+      </c>
+      <c r="C179" t="n">
+        <v>0.4960528753410618</v>
+      </c>
+      <c r="D179" t="n">
+        <v>1</v>
+      </c>
+      <c r="E179" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="n">
+        <v>0.7021276595744681</v>
+      </c>
+      <c r="C180" t="n">
+        <v>0.462267267743469</v>
+      </c>
+      <c r="D180" t="n">
+        <v>1</v>
+      </c>
+      <c r="E180" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="n">
+        <v>1.531914893617021</v>
+      </c>
+      <c r="C181" t="n">
+        <v>1.018333332071646</v>
+      </c>
+      <c r="D181" t="n">
+        <v>1</v>
+      </c>
+      <c r="E181" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="n">
+        <v>0.5319148936170213</v>
+      </c>
+      <c r="C182" t="n">
+        <v>0.5043749394606821</v>
+      </c>
+      <c r="D182" t="n">
+        <v>1</v>
+      </c>
+      <c r="E182" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="n">
+        <v>0.6170212765957447</v>
+      </c>
+      <c r="C183" t="n">
+        <v>0.4913686072930561</v>
+      </c>
+      <c r="D183" t="n">
+        <v>1</v>
+      </c>
+      <c r="E183" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="C184" t="n">
+        <v>1.312784923481051</v>
+      </c>
+      <c r="D184" t="n">
+        <v>1</v>
+      </c>
+      <c r="E184" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C185" t="n">
+        <v>0.4892460547900817</v>
+      </c>
+      <c r="D185" t="n">
+        <v>1</v>
+      </c>
+      <c r="E185" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C186" t="n">
+        <v>0.4375949744936837</v>
+      </c>
+      <c r="D186" t="n">
+        <v>1</v>
+      </c>
+      <c r="E186" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="n">
+        <v>0.04359753086419754</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0.04098396935177413</v>
+      </c>
+      <c r="D187" t="n">
+        <v>4</v>
+      </c>
+      <c r="E187" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="n">
+        <v>0.3733296296296297</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0.1147026987961099</v>
+      </c>
+      <c r="D188" t="n">
+        <v>4</v>
+      </c>
+      <c r="E188" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="n">
+        <v>0.7609024691358024</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0.2068526528566341</v>
+      </c>
+      <c r="D189" t="n">
+        <v>4</v>
+      </c>
+      <c r="E189" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="n">
+        <v>0.1236896551724138</v>
+      </c>
+      <c r="C190" t="n">
+        <v>0.1006976036912625</v>
+      </c>
+      <c r="D190" t="n">
+        <v>3</v>
+      </c>
+      <c r="E190" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="n">
+        <v>2.782674516400336</v>
+      </c>
+      <c r="C191" t="n">
+        <v>2.456039114421036</v>
+      </c>
+      <c r="D191" t="n">
+        <v>18</v>
+      </c>
+      <c r="E191" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="n">
+        <v>1.0257</v>
+      </c>
+      <c r="C192" t="n">
+        <v>0.466632716209156</v>
+      </c>
+      <c r="D192" t="n">
+        <v>3</v>
+      </c>
+      <c r="E192" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="n">
+        <v>0.3695000000000001</v>
+      </c>
+      <c r="C193" t="n">
+        <v>0.1165490612294642</v>
+      </c>
+      <c r="D193" t="n">
+        <v>3</v>
+      </c>
+      <c r="E193" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="n">
+        <v>3.48552</v>
+      </c>
+      <c r="C194" t="n">
+        <v>1.096076011068948</v>
+      </c>
+      <c r="D194" t="n">
+        <v>3</v>
+      </c>
+      <c r="E194" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="n">
+        <v>660.6794871794872</v>
+      </c>
+      <c r="C195" t="n">
+        <v>89.62468548945792</v>
+      </c>
+      <c r="D195" t="n">
+        <v>1</v>
+      </c>
+      <c r="E195" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="n">
+        <v>92.25641025641026</v>
+      </c>
+      <c r="C196" t="n">
+        <v>11.3954147732971</v>
+      </c>
+      <c r="D196" t="n">
+        <v>1</v>
+      </c>
+      <c r="E196" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="n">
+        <v>96.37948717948717</v>
+      </c>
+      <c r="C197" t="n">
+        <v>1.150308707786794</v>
+      </c>
+      <c r="D197" t="n">
+        <v>1</v>
+      </c>
+      <c r="E197" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="n">
+        <v>3.499999999999999</v>
+      </c>
+      <c r="C198" t="n">
+        <v>1.522557656767657</v>
+      </c>
+      <c r="D198" t="n">
+        <v>1</v>
+      </c>
+      <c r="E198" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="n">
+        <v>36.06410256410256</v>
+      </c>
+      <c r="C199" t="n">
+        <v>11.94722131862038</v>
+      </c>
+      <c r="D199" t="n">
+        <v>1</v>
+      </c>
+      <c r="E199" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="n">
+        <v>-7.773076923076922</v>
+      </c>
+      <c r="C200" t="n">
+        <v>13.13981431679003</v>
+      </c>
+      <c r="D200" t="n">
+        <v>1</v>
+      </c>
+      <c r="E200" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="n">
+        <v>33.64102564102564</v>
+      </c>
+      <c r="C202" t="n">
+        <v>2.125750342541315</v>
+      </c>
+      <c r="D202" t="n">
+        <v>1</v>
+      </c>
+      <c r="E202" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="n">
+        <v>278.6153846153846</v>
+      </c>
+      <c r="C203" t="n">
+        <v>201.146081875204</v>
+      </c>
+      <c r="D203" t="n">
+        <v>1</v>
+      </c>
+      <c r="E203" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="n">
+        <v>-14.28717948717948</v>
+      </c>
+      <c r="C204" t="n">
+        <v>16.08104764124817</v>
+      </c>
+      <c r="D204" t="n">
+        <v>1</v>
+      </c>
+      <c r="E204" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="n">
+        <v>7.629487179487181</v>
+      </c>
+      <c r="C205" t="n">
+        <v>0.8332550745804188</v>
+      </c>
+      <c r="D205" t="n">
+        <v>1</v>
+      </c>
+      <c r="E205" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="n">
+        <v>9.694871794871796</v>
+      </c>
+      <c r="C206" t="n">
+        <v>2.402536399761958</v>
+      </c>
+      <c r="D206" t="n">
+        <v>1</v>
+      </c>
+      <c r="E206" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="n">
+        <v>25.0076923076923</v>
+      </c>
+      <c r="C207" t="n">
+        <v>12.24299183822521</v>
+      </c>
+      <c r="D207" t="n">
+        <v>1</v>
+      </c>
+      <c r="E207" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="n">
+        <v>-0.8782051282051282</v>
+      </c>
+      <c r="C208" t="n">
+        <v>0.2789811872340192</v>
+      </c>
+      <c r="D208" t="n">
+        <v>1</v>
+      </c>
+      <c r="E208" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="n">
+        <v>264.448717948718</v>
+      </c>
+      <c r="C209" t="n">
+        <v>21.43285948881917</v>
+      </c>
+      <c r="D209" t="n">
+        <v>1</v>
+      </c>
+      <c r="E209" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="n">
+        <v>109.5769230769231</v>
+      </c>
+      <c r="C210" t="n">
+        <v>10.96336192485246</v>
+      </c>
+      <c r="D210" t="n">
+        <v>1</v>
+      </c>
+      <c r="E210" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="n">
+        <v>199.3076923076923</v>
+      </c>
+      <c r="C211" t="n">
+        <v>20.00669218705912</v>
+      </c>
+      <c r="D211" t="n">
+        <v>1</v>
+      </c>
+      <c r="E211" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="n">
+        <v>89.73076923076923</v>
+      </c>
+      <c r="C212" t="n">
+        <v>19.6545973452319</v>
+      </c>
+      <c r="D212" t="n">
+        <v>1</v>
+      </c>
+      <c r="E212" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="n">
+        <v>124.2179487179487</v>
+      </c>
+      <c r="C213" t="n">
+        <v>106.8728638350682</v>
+      </c>
+      <c r="D213" t="n">
+        <v>1</v>
+      </c>
+      <c r="E213" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="n">
+        <v>35.05128205128205</v>
+      </c>
+      <c r="C214" t="n">
+        <v>4.044869881834564</v>
+      </c>
+      <c r="D214" t="n">
+        <v>1</v>
+      </c>
+      <c r="E214" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>698.453846153846</v>
+      </c>
+      <c r="C215" t="n">
+        <v>59.69679817450608</v>
+      </c>
+      <c r="D215" t="n">
+        <v>1</v>
+      </c>
+      <c r="E215" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>3.360384615384616</v>
+      </c>
+      <c r="C216" t="n">
+        <v>1.027253863220041</v>
+      </c>
+      <c r="D216" t="n">
+        <v>2</v>
+      </c>
+      <c r="E216" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>0</v>
+      </c>
+      <c r="C217" t="n">
+        <v>0</v>
+      </c>
+      <c r="D217" t="n">
+        <v>1</v>
+      </c>
+      <c r="E217" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>